<commit_message>
colocar a estrutura dos docs
</commit_message>
<xml_diff>
--- a/doc_strutucture.xlsx
+++ b/doc_strutucture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufpebr0-my.sharepoint.com/personal/marcus_torres_ufpe_br/Documents/UFPE/DOUTORADO/dynastiesBR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{C78D0818-CDBA-4870-87C3-7B5C6F709355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{914FF961-B194-4A0B-8E14-89A1C75E2F50}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{C78D0818-CDBA-4870-87C3-7B5C6F709355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A190F550-DDF5-4AD9-B749-937C233F0E16}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{176FE2DB-701A-4519-BDE4-912EA31D2C78}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="146">
   <si>
     <t>UF</t>
   </si>
@@ -460,6 +460,9 @@
   </si>
   <si>
     <t>https://divulgacandcontas.tse.jus.br/candidaturas/oficial/2020/MG/41238/426/candidatos/289933/15_1600126854656.pdf</t>
+  </si>
+  <si>
+    <t>FILIAÇAO 1:/n FILIAÇAO 2</t>
   </si>
 </sst>
 </file>
@@ -826,11 +829,14 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="A2:O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1505,6 +1511,9 @@
       </c>
       <c r="L21">
         <v>2</v>
+      </c>
+      <c r="M21" t="s">
+        <v>145</v>
       </c>
       <c r="N21" t="s">
         <v>34</v>

</xml_diff>